<commit_message>
Add off switch GPIO.
</commit_message>
<xml_diff>
--- a/SBC_IO.xlsx
+++ b/SBC_IO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwest\Dropbox (Planetary Power)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwest\dev\HyGenCMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="246">
   <si>
     <t>Beaglebone IO</t>
   </si>
@@ -758,6 +758,12 @@
   </si>
   <si>
     <t>Pulse_A2D (additional input)</t>
+  </si>
+  <si>
+    <t>gpio0[22]</t>
+  </si>
+  <si>
+    <t>OFF switch</t>
   </si>
 </sst>
 </file>
@@ -1440,8 +1446,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,9 +1897,15 @@
       <c r="A20" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="9">
+        <v>7</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>245</v>
+      </c>
       <c r="F20" s="14" t="s">
         <v>207</v>
       </c>

</xml_diff>

<commit_message>
Enable poweroff option from GPIO signal on P8_19
</commit_message>
<xml_diff>
--- a/SBC_IO.xlsx
+++ b/SBC_IO.xlsx
@@ -1447,7 +1447,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,7 +2352,7 @@
         <v>63</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -2378,7 +2378,7 @@
         <v>64</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2403,7 +2403,6 @@
       <c r="H41" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">

</xml_diff>